<commit_message>
hys 2 day 2
</commit_message>
<xml_diff>
--- a/data-raw/HYS2/HYS2.xlsx
+++ b/data-raw/HYS2/HYS2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="103">
   <si>
     <t>well</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>day1</t>
+  </si>
+  <si>
+    <t>day2</t>
   </si>
 </sst>
 </file>
@@ -1422,6 +1425,9 @@
       <c r="C1" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
@@ -1433,7 +1439,9 @@
       <c r="C2" s="5">
         <v>0.13279999792575836</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="5">
+        <v>0.28189998865127563</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1455,6 +1463,9 @@
       <c r="C3" s="7">
         <v>0.04899999871850014</v>
       </c>
+      <c r="D3" s="7">
+        <v>0.05119999870657921</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
@@ -1466,6 +1477,9 @@
       <c r="C4" s="7">
         <v>0.1273999959230423</v>
       </c>
+      <c r="D4" s="7">
+        <v>0.30640000104904175</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
@@ -1477,6 +1491,9 @@
       <c r="C5" s="7">
         <v>0.1340000033378601</v>
       </c>
+      <c r="D5" s="7">
+        <v>0.3197999894618988</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
@@ -1488,6 +1505,9 @@
       <c r="C6" s="7">
         <v>0.3084999918937683</v>
       </c>
+      <c r="D6" s="7">
+        <v>0.16899999976158142</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
@@ -1499,6 +1519,9 @@
       <c r="C7" s="7">
         <v>0.27570000290870667</v>
       </c>
+      <c r="D7" s="7">
+        <v>0.1623000055551529</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
@@ -1510,6 +1533,9 @@
       <c r="C8" s="7">
         <v>0.22300000488758087</v>
       </c>
+      <c r="D8" s="7">
+        <v>0.09920000284910202</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
@@ -1521,6 +1547,9 @@
       <c r="C9" s="7">
         <v>0.050599999725818634</v>
       </c>
+      <c r="D9" s="7">
+        <v>0.04989999905228615</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
@@ -1532,6 +1561,9 @@
       <c r="C10" s="7">
         <v>0.1589999943971634</v>
       </c>
+      <c r="D10" s="7">
+        <v>0.16269999742507935</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
@@ -1543,6 +1575,9 @@
       <c r="C11" s="7">
         <v>0.16349999606609344</v>
       </c>
+      <c r="D11" s="7">
+        <v>0.14010000228881836</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
@@ -1554,6 +1589,9 @@
       <c r="C12" s="7">
         <v>0.04899999871850014</v>
       </c>
+      <c r="D12" s="7">
+        <v>0.053199999034404755</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
@@ -1565,6 +1603,9 @@
       <c r="C13" s="7">
         <v>0.13420000672340393</v>
       </c>
+      <c r="D13" s="7">
+        <v>0.10840000212192535</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -1576,6 +1617,9 @@
       <c r="C14" s="7">
         <v>0.05009999871253967</v>
       </c>
+      <c r="D14" s="7">
+        <v>0.04769999906420708</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
@@ -1587,6 +1631,9 @@
       <c r="C15" s="7">
         <v>0.14329999685287476</v>
       </c>
+      <c r="D15" s="7">
+        <v>0.3425999879837036</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
@@ -1598,6 +1645,9 @@
       <c r="C16" s="7">
         <v>0.1354999989271164</v>
       </c>
+      <c r="D16" s="7">
+        <v>0.28110000491142273</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
@@ -1609,6 +1659,9 @@
       <c r="C17" s="7">
         <v>0.13930000364780426</v>
       </c>
+      <c r="D17" s="7">
+        <v>0.2694000005722046</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
@@ -1620,6 +1673,9 @@
       <c r="C18" s="7">
         <v>0.20360000431537628</v>
       </c>
+      <c r="D18" s="7">
+        <v>0.3303000032901764</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
@@ -1631,6 +1687,9 @@
       <c r="C19" s="7">
         <v>0.21160000562667847</v>
       </c>
+      <c r="D19" s="7">
+        <v>0.11079999804496765</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
@@ -1642,6 +1701,9 @@
       <c r="C20" s="7">
         <v>0.21649999916553497</v>
       </c>
+      <c r="D20" s="7">
+        <v>0.1875</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
@@ -1653,6 +1715,9 @@
       <c r="C21" s="7">
         <v>0.04969999939203262</v>
       </c>
+      <c r="D21" s="7">
+        <v>0.053300000727176666</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
@@ -1664,6 +1729,9 @@
       <c r="C22" s="7">
         <v>0.21299999952316284</v>
       </c>
+      <c r="D22" s="7">
+        <v>0.423799991607666</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
@@ -1675,6 +1743,9 @@
       <c r="C23" s="7">
         <v>0.04989999905228615</v>
       </c>
+      <c r="D23" s="7">
+        <v>0.05119999870657921</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
@@ -1686,6 +1757,9 @@
       <c r="C24" s="7">
         <v>0.2410999983549118</v>
       </c>
+      <c r="D24" s="7">
+        <v>0.31299999356269836</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
@@ -1696,6 +1770,9 @@
       </c>
       <c r="C25" s="7">
         <v>0.22130000591278076</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.15690000355243683</v>
       </c>
     </row>
   </sheetData>
@@ -1723,6 +1800,9 @@
       <c r="C1" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
@@ -1734,6 +1814,9 @@
       <c r="C2" s="7">
         <v>0.05979999899864197</v>
       </c>
+      <c r="D2" s="7">
+        <v>0.050200000405311584</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
@@ -1745,6 +1828,9 @@
       <c r="C3" s="7">
         <v>0.05209999904036522</v>
       </c>
+      <c r="D3" s="7">
+        <v>0.050999999046325684</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
@@ -1756,6 +1842,9 @@
       <c r="C4" s="7">
         <v>0.05739999935030937</v>
       </c>
+      <c r="D4" s="7">
+        <v>0.05130000039935112</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
@@ -1767,6 +1856,9 @@
       <c r="C5" s="7">
         <v>0.05779999867081642</v>
       </c>
+      <c r="D5" s="7">
+        <v>0.05040000006556511</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
@@ -1778,6 +1870,9 @@
       <c r="C6" s="7">
         <v>0.057999998331069946</v>
       </c>
+      <c r="D6" s="7">
+        <v>0.050700001418590546</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
@@ -1789,6 +1884,9 @@
       <c r="C7" s="7">
         <v>0.05900000035762787</v>
       </c>
+      <c r="D7" s="7">
+        <v>0.04969999939203262</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
@@ -1800,6 +1898,9 @@
       <c r="C8" s="7">
         <v>0.0568000003695488</v>
       </c>
+      <c r="D8" s="7">
+        <v>0.05139999836683273</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
@@ -1811,6 +1912,9 @@
       <c r="C9" s="7">
         <v>0.05380000174045563</v>
       </c>
+      <c r="D9" s="7">
+        <v>0.05299999937415123</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
@@ -1822,6 +1926,9 @@
       <c r="C10" s="7">
         <v>0.059300001710653305</v>
       </c>
+      <c r="D10" s="7">
+        <v>0.05009999871253967</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
@@ -1833,6 +1940,9 @@
       <c r="C11" s="7">
         <v>0.05660000070929527</v>
       </c>
+      <c r="D11" s="7">
+        <v>0.048700001090765</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
@@ -1844,6 +1954,9 @@
       <c r="C12" s="7">
         <v>0.04839999973773956</v>
       </c>
+      <c r="D12" s="7">
+        <v>0.0478999987244606</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
@@ -1855,6 +1968,9 @@
       <c r="C13" s="7">
         <v>0.05460000038146973</v>
       </c>
+      <c r="D13" s="7">
+        <v>0.04859999939799309</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -1866,6 +1982,9 @@
       <c r="C14" s="7">
         <v>0.049800001084804535</v>
       </c>
+      <c r="D14" s="7">
+        <v>0.04479999840259552</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
@@ -1877,6 +1996,9 @@
       <c r="C15" s="7">
         <v>0.060499999672174454</v>
       </c>
+      <c r="D15" s="7">
+        <v>0.04500000178813934</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
@@ -1888,6 +2010,9 @@
       <c r="C16" s="7">
         <v>0.05999999865889549</v>
       </c>
+      <c r="D16" s="7">
+        <v>0.04800000041723251</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
@@ -1899,6 +2024,9 @@
       <c r="C17" s="7">
         <v>0.060499999672174454</v>
       </c>
+      <c r="D17" s="7">
+        <v>0.04540000110864639</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
@@ -1910,6 +2038,9 @@
       <c r="C18" s="7">
         <v>0.060600001364946365</v>
       </c>
+      <c r="D18" s="7">
+        <v>0.05139999836683273</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
@@ -1921,6 +2052,9 @@
       <c r="C19" s="7">
         <v>0.0575999990105629</v>
       </c>
+      <c r="D19" s="7">
+        <v>0.05009999871253967</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
@@ -1932,6 +2066,9 @@
       <c r="C20" s="7">
         <v>0.05640000104904175</v>
       </c>
+      <c r="D20" s="7">
+        <v>0.0494999997317791</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
@@ -1943,6 +2080,9 @@
       <c r="C21" s="7">
         <v>0.05169999971985817</v>
       </c>
+      <c r="D21" s="7">
+        <v>0.048500001430511475</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
@@ -1954,6 +2094,9 @@
       <c r="C22" s="7">
         <v>0.061799999326467514</v>
       </c>
+      <c r="D22" s="7">
+        <v>0.04540000110864639</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
@@ -1965,6 +2108,9 @@
       <c r="C23" s="7">
         <v>0.05169999971985817</v>
       </c>
+      <c r="D23" s="7">
+        <v>0.04540000110864639</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
@@ -1976,6 +2122,9 @@
       <c r="C24" s="7">
         <v>0.06669999659061432</v>
       </c>
+      <c r="D24" s="7">
+        <v>0.04650000110268593</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
@@ -1986,6 +2135,9 @@
       </c>
       <c r="C25" s="7">
         <v>0.06310000270605087</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.045899998396635056</v>
       </c>
     </row>
     <row r="26">

</xml_diff>

<commit_message>
hys2 day 3 raw data
</commit_message>
<xml_diff>
--- a/data-raw/HYS2/HYS2.xlsx
+++ b/data-raw/HYS2/HYS2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="106">
   <si>
     <t>well</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>day3</t>
   </si>
 </sst>
 </file>
@@ -2492,6 +2495,342 @@
         <v>102</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.22579999268054962</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.05000000074505806</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.24789999425411224</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.15620000660419464</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0.2110999971628189</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="7">
+        <v>0.20970000326633453</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0.2134000062942505</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0.0478999987244606</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0.23469999432563782</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0.3447999954223633</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0.04899999871850014</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0.3109000027179718</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.05400000140070915</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0.17730000615119934</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0.20909999310970306</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0.163100004196167</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.2069000005722046</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0.22360000014305115</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0.25110000371932983</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0.05090000107884407</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="7">
+        <v>0.28380000591278076</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" s="7">
+        <v>0.05050000175833702</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="7">
+        <v>0.2547999918460846</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="7">
+        <v>0.22859999537467957</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3579,6 +3918,342 @@
         <v>102</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.05220000073313713</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.051500000059604645</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.050599999725818634</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.050200000405311584</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0.04969999939203262</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="7">
+        <v>0.0478999987244606</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0.050200000405311584</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0.051600001752376556</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0.0502999983727932</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0.048900000751018524</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0.04820000007748604</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0.051100000739097595</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.04919999837875366</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0.049300000071525574</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0.04910000041127205</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0.04989999905228615</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.05119999870657921</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0.050200000405311584</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0.048700001090765</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0.0494999997317791</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="7">
+        <v>0.04910000041127205</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" s="7">
+        <v>0.04989999905228615</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" s="7">
+        <v>0.050599999725818634</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="7">
+        <v>0.05350000038743019</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>